<commit_message>
For deposit at Debuz
</commit_message>
<xml_diff>
--- a/Time Table June  2018.xlsx
+++ b/Time Table June  2018.xlsx
@@ -6484,16 +6484,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>180703</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>444136</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>30479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>195944</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>421276</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>7618</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6502,7 +6502,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14789332" y="11601993"/>
+          <a:off x="16117389" y="11634650"/>
           <a:ext cx="679269" cy="423454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7282,16 +7282,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>469175</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>447405</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>433251</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>232954</xdr:colOff>
+      <xdr:rowOff>444136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>211184</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>410391</xdr:rowOff>
+      <xdr:rowOff>421276</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7300,7 +7300,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14413775" y="11591108"/>
+          <a:off x="15720062" y="11601993"/>
           <a:ext cx="427808" cy="423454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -18604,13 +18604,86 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>ผ่านมือถือ ที่มหาลัย</a:t>
+            <a:t>ที่บ้าน</a:t>
           </a:r>
           <a:endParaRPr>
             <a:solidFill>
               <a:schemeClr val="bg1"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>468088</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>391885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>587829</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="395" name="สี่เหลี่ยมผืนผ้า 394"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13748659" y="11549742"/>
+          <a:ext cx="2111827" cy="533401"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="900"/>
+            <a:t>ศึกษารายจ่ายทั้งหมดของ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="900"/>
+            <a:t>Osaka</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="900"/>
+            <a:t>บอกแม่ด้วยว่า จะรีบจ่ายค่าโรงแรม กับค่าเครื่องบิน ก่อนที่มันจะแพงกว่านี้</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -18908,8 +18981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added the report taking picture adding
</commit_message>
<xml_diff>
--- a/Time Table June  2018.xlsx
+++ b/Time Table June  2018.xlsx
@@ -18065,7 +18065,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>642257</xdr:colOff>
+      <xdr:colOff>370115</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>413658</xdr:rowOff>
     </xdr:from>
@@ -18082,8 +18082,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3298371" y="15142029"/>
-          <a:ext cx="674914" cy="403440"/>
+          <a:off x="3026229" y="15142029"/>
+          <a:ext cx="947056" cy="403440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18110,7 +18110,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1000">
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:schemeClr val="bg1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
@@ -18118,21 +18118,24 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000">
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:schemeClr val="bg1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>ฝาก</a:t>
-          </a:r>
-          <a:endParaRPr/>
+            <a:t>เอากลับมา</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -18684,6 +18687,371 @@
             <a:rPr lang="th-TH" sz="900"/>
             <a:t>บอกแม่ด้วยว่า จะรีบจ่ายค่าโรงแรม กับค่าเครื่องบิน ก่อนที่มันจะแพงกว่านี้</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>315685</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>32659</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>239488</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>348343</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="396" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16252371" y="15207345"/>
+          <a:ext cx="1251860" cy="315684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>erect dom</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>326571</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>21774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>402774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="397" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8958942" y="16535403"/>
+          <a:ext cx="2481945" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>relax</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>32660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>130629</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>413660</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="398" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8937170" y="16992603"/>
+          <a:ext cx="2481945" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>relax</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>293913</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>402772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>65316</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="399" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4942113" y="15577458"/>
+          <a:ext cx="1099458" cy="555172"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>เอาปลากระป๋องแห้งไปทานมื้อเทียงด้วย</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>21773</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>435428</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="400" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7990116" y="15773401"/>
+          <a:ext cx="3831770" cy="283027"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ถ่ายภาพ ทำ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Report </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>รายงานผลสหกิจ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ถามพี่เลี้ยง อันนี้</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -18981,8 +19349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ugh, need more exercises and travel, and relax more, and be awesome as well
</commit_message>
<xml_diff>
--- a/Time Table June  2018.xlsx
+++ b/Time Table June  2018.xlsx
@@ -15321,16 +15321,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>598715</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>446312</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>435430</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>423451</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>25034</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>642256</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>9794</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -15339,8 +15339,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11223172" y="12050483"/>
-          <a:ext cx="1164772" cy="423454"/>
+          <a:off x="6281057" y="16984977"/>
+          <a:ext cx="1665513" cy="431074"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15378,7 +15378,13 @@
             <a:rPr lang="en-US" sz="1000"/>
             <a:t> Law of existence</a:t>
           </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เอาจริงละ</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -18622,13 +18628,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>468088</xdr:colOff>
+      <xdr:colOff>402774</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>391885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>587829</xdr:colOff>
+      <xdr:colOff>522515</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>32657</xdr:rowOff>
     </xdr:to>
@@ -18639,7 +18645,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13748659" y="11549742"/>
+          <a:off x="13683345" y="11549742"/>
           <a:ext cx="2111827" cy="533401"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -18762,25 +18768,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>326571</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>21774</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>402774</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="397" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8958942" y="16535403"/>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>32660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>370116</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>413660</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="398" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8512628" y="16992603"/>
           <a:ext cx="2481945" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -18830,25 +18836,786 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>293913</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>402772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>65316</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="399" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4942113" y="15577458"/>
+          <a:ext cx="1099458" cy="555172"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>เอาปลากระป๋องแห้งไปทานมื้อเทียงด้วย</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>21773</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>435428</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="400" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7990116" y="15773401"/>
+          <a:ext cx="3831770" cy="283027"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ถ่ายภาพ ทำ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Report </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>รายงานผลสหกิจ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ถามพี่เลี้ยง อันนี้</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>32658</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>413659</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="401" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6640286" y="18756087"/>
+          <a:ext cx="6008915" cy="402772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>สหกิจ</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>21773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>424545</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="402" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6662057" y="19213287"/>
+          <a:ext cx="6008915" cy="402772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>สหกิจ</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>413658</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="403" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6662057" y="19648715"/>
+          <a:ext cx="6008915" cy="402772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>สหกิจ</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>32657</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>65315</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>413659</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="404" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6672943" y="20095030"/>
+          <a:ext cx="6008915" cy="402772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>สหกิจ</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>10888</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>413660</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="405" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6651171" y="20541345"/>
+          <a:ext cx="6008915" cy="402772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>สหกิจ</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>555172</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>570412</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>419099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="408" name="สี่เหลี่ยมผืนผ้า 407"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11843658" y="16513628"/>
+          <a:ext cx="679268" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ออกกำลัง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>576944</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>435428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>592183</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>408214</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="409" name="สี่เหลี่ยมผืนผ้า 408"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11201401" y="18734314"/>
+          <a:ext cx="679268" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ออกกำลัง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>598716</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>613955</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>429986</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="410" name="สี่เหลี่ยมผืนผ้า 409"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11223173" y="19648715"/>
+          <a:ext cx="679268" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ออกกำลัง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>620488</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>635727</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>5444</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="411" name="สี่เหลี่ยมผืนผ้า 410"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11244945" y="20563115"/>
+          <a:ext cx="679268" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ออกกำลัง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>631373</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>646612</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>440872</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="412" name="สี่เหลี่ยมผืนผ้า 411"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11255830" y="21444858"/>
+          <a:ext cx="679268" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ออกกำลัง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>250371</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>21774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>32660</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>130629</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>413660</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="398" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8937170" y="16992603"/>
+      <xdr:colOff>76202</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>402774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="413" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6226628" y="16535403"/>
           <a:ext cx="2481945" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -18880,7 +19647,34 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>relax</a:t>
+            <a:t>relax </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ไปชมรม</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>เล่นอสุราต่อ</a:t>
           </a:r>
           <a:endParaRPr/>
         </a:p>
@@ -18898,35 +19692,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>293913</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>402772</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>65314</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>65316</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="399" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4942113" y="15577458"/>
-          <a:ext cx="1099458" cy="555172"/>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>43546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>544287</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>424546</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="414" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8686799" y="16557175"/>
+          <a:ext cx="2481945" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
+          <a:srgbClr val="00B050"/>
         </a:solidFill>
         <a:ln w="25560">
           <a:solidFill>
@@ -18939,24 +19730,151 @@
         <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
         <a:lstStyle/>
         <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ที่ชมรม ขอข้อมูลค่าใช้จ่าย การใช้ชีวิต เที่ยวญี่ปุ่น</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:pPr>
             <a:lnSpc>
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="th-TH">
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>576943</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>446313</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>592183</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>419099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="415" name="สี่เหลี่ยมผืนผ้า 414"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11865429" y="16959942"/>
+          <a:ext cx="679268" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ออกกำลัง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76202</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>751117</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>391886</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="416" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16764000" y="16143516"/>
+          <a:ext cx="1251860" cy="315684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
-                <a:schemeClr val="bg1"/>
+                <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
+              <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>เอาปลากระป๋องแห้งไปทานมื้อเทียงด้วย</a:t>
-          </a:r>
-          <a:endParaRPr>
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
+            <a:t>erect sub</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -18964,25 +19882,161 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>21773</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>435428</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="400" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7990116" y="15773401"/>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>337457</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>65316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>925288</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="417" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16938171" y="16578945"/>
+          <a:ext cx="1251860" cy="315684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>erect sub</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>108859</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>892631</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>424543</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="418" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16905514" y="17068802"/>
+          <a:ext cx="1251860" cy="315684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>erect dom</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>566059</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>174172</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>413658</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="419" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7206345" y="18919372"/>
           <a:ext cx="3831770" cy="283027"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -19052,6 +20106,749 @@
               <a:schemeClr val="bg1"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>315687</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="420" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12932230" y="17569542"/>
+          <a:ext cx="4593770" cy="424543"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>วันหยุด</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> ห้าม</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>!!! </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ทำงานถ้าไม่จำเป็นจริงๆ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ไม่งั้นมันจะเครียดจนยิ่งทำงานไม่ได้</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>กันไว้ดีกว่าแก้ กันโง่ไว้</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>315686</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>10889</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>141517</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>391889</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="421" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6291943" y="20987660"/>
+          <a:ext cx="2481945" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>relax </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ไปชมรม</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>เล่นอสุราต่อ</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>174171</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>391889</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>326575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="422" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8806542" y="20922346"/>
+          <a:ext cx="2481945" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ที่ชมรม ขอข้อมูลค่าใช้จ่าย การใช้ชีวิต เที่ยวญี่ปุ่น</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>54427</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>65316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="423" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6694713" y="21488402"/>
+          <a:ext cx="4082144" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>เที่ยว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Japan Town</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>653143</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>413657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>370783</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="424" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3309257" y="18712543"/>
+          <a:ext cx="674914" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ฝาก</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>620486</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>435429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>631371</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>392554</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="425" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3276600" y="19626943"/>
+          <a:ext cx="674914" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ฝาก</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>424544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>631370</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>381670</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="426" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3004457" y="19169744"/>
+          <a:ext cx="947056" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>เอากลับมา</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>326572</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>435430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>392556</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="427" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2982686" y="20519573"/>
+          <a:ext cx="947056" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>เอากลับมา</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>576943</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>424544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>587828</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>381670</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="428" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3233057" y="20062373"/>
+          <a:ext cx="674914" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ฝาก</a:t>
+          </a:r>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -19349,8 +21146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S38" sqref="S38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
social improvement magic and truth
</commit_message>
<xml_diff>
--- a/Time Table June  2018.xlsx
+++ b/Time Table June  2018.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -19473,16 +19472,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>631373</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304802</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>21772</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>646612</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>440872</xdr:rowOff>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>320041</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>5444</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -19491,7 +19490,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11255830" y="21444858"/>
+          <a:off x="12257316" y="21455744"/>
           <a:ext cx="679268" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -20261,16 +20260,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>54427</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>370113</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>65316</xdr:rowOff>
+      <xdr:rowOff>43544</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
+      <xdr:colOff>359228</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>424544</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -20279,8 +20278,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6694713" y="21488402"/>
-          <a:ext cx="4082144" cy="381000"/>
+          <a:off x="7674427" y="21466630"/>
+          <a:ext cx="3309258" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20306,7 +20305,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>เที่ยว </a:t>
+            <a:t>เที่ยว</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100">
@@ -20315,7 +20314,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Japan Town</a:t>
+            <a:t> MBK</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH">
             <a:effectLst/>
@@ -21655,16 +21654,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>119741</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>435427</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>89262</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>326569</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>408212</xdr:rowOff>
+      <xdr:rowOff>101235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>296090</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>81641</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -21673,8 +21672,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5431970" y="21412198"/>
-          <a:ext cx="633549" cy="419100"/>
+          <a:off x="6966855" y="21524321"/>
+          <a:ext cx="633549" cy="426720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -22701,6 +22700,71 @@
             <a:t>pone</a:t>
           </a:r>
           <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>359228</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>293914</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>435429</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="456" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10319657" y="21477515"/>
+          <a:ext cx="1926771" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ไปมหาลัย</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -23007,7 +23071,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R50" sqref="R50"/>
+      <selection activeCell="U51" sqref="U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>